<commit_message>
Adding Austria and Switzerland, enabling district heating and industrial steam for the NT2030 and NT2040
</commit_message>
<xml_diff>
--- a/src_files/data_files/balticData.xlsx
+++ b/src_files/data_files/balticData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backbone\backbone\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1795513D-ADB2-424D-AA13-657FE0A593ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B11B6F-D5D2-4466-B9FE-5365131C2089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitdata_Baltic" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Bio CHP</t>
   </si>
   <si>
-    <t>National Trends</t>
-  </si>
-  <si>
     <t>unit_name_prefix</t>
   </si>
   <si>
@@ -373,6 +370,9 @@
   </si>
   <si>
     <t>Unit type added</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -710,6 +710,12 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,8 +1003,8 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,8 +1012,8 @@
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17" style="34" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="34" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="13" max="13" width="19.5703125" customWidth="1"/>
@@ -1021,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1033,22 +1039,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>6</v>
@@ -1062,11 +1068,11 @@
         <v>8</v>
       </c>
       <c r="C2" s="32"/>
-      <c r="D2" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="32">
-        <v>2025</v>
+      <c r="D2" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="33">
+        <v>1</v>
       </c>
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
@@ -1090,14 +1096,14 @@
         <v>7</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="32"/>
-      <c r="D3" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="32">
-        <v>2025</v>
+      <c r="D3" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="33">
+        <v>1</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
@@ -1121,14 +1127,14 @@
         <v>7</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="32"/>
-      <c r="D4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="32">
-        <v>2025</v>
+      <c r="D4" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="33">
+        <v>1</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32"/>
@@ -1152,14 +1158,14 @@
         <v>7</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="32"/>
-      <c r="D5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="32">
-        <v>2025</v>
+      <c r="D5" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="33">
+        <v>1</v>
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="32"/>
@@ -1180,14 +1186,14 @@
         <v>7</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="32"/>
-      <c r="D6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="32">
-        <v>2025</v>
+      <c r="D6" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="33">
+        <v>1</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32"/>
@@ -1208,14 +1214,14 @@
         <v>7</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="32"/>
-      <c r="D7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="32">
-        <v>2025</v>
+      <c r="D7" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="33">
+        <v>1</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
@@ -1236,14 +1242,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="32"/>
-      <c r="D8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="32">
-        <v>2025</v>
+      <c r="D8" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="33">
+        <v>1</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
@@ -1263,14 +1269,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="32"/>
-      <c r="D9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="32">
-        <v>2025</v>
+      <c r="D9" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="33">
+        <v>1</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
@@ -1287,17 +1293,17 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="32"/>
-      <c r="D10" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="32">
-        <v>2025</v>
+      <c r="D10" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="33">
+        <v>1</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -1318,17 +1324,17 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="32">
-        <v>2025</v>
+      <c r="D11" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="33">
+        <v>1</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
@@ -1349,17 +1355,17 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="32"/>
-      <c r="D12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="32">
-        <v>2025</v>
+      <c r="D12" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="33">
+        <v>1</v>
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
@@ -1380,17 +1386,17 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="32"/>
-      <c r="D13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="32">
-        <v>2025</v>
+      <c r="D13" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="33">
+        <v>1</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
@@ -1408,17 +1414,17 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="32"/>
-      <c r="D14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="32">
-        <v>2025</v>
+      <c r="D14" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="33">
+        <v>1</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
@@ -1436,17 +1442,17 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="32"/>
-      <c r="D15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="32">
-        <v>2025</v>
+      <c r="D15" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="33">
+        <v>1</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
@@ -1464,17 +1470,17 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="32"/>
-      <c r="D16" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="32">
-        <v>2025</v>
+      <c r="D16" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="33">
+        <v>1</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
@@ -1491,17 +1497,17 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="32">
-        <v>2025</v>
+      <c r="D17" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="33">
+        <v>1</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="32"/>
@@ -1518,17 +1524,17 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="32"/>
-      <c r="D18" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="32">
-        <v>2025</v>
+      <c r="D18" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="33">
+        <v>1</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
@@ -1549,17 +1555,17 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="32"/>
-      <c r="D19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="32">
-        <v>2025</v>
+      <c r="D19" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="33">
+        <v>1</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="32"/>
@@ -1580,17 +1586,17 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>22</v>
-      </c>
       <c r="C20" s="32"/>
-      <c r="D20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="32">
-        <v>2025</v>
+      <c r="D20" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="33">
+        <v>1</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
@@ -1609,22 +1615,22 @@
         <v>1.34375</v>
       </c>
       <c r="M20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="32"/>
-      <c r="D21" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="32">
-        <v>2025</v>
+      <c r="D21" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="33">
+        <v>1</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="32"/>
@@ -1645,17 +1651,17 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="32"/>
-      <c r="D22" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="32">
-        <v>2025</v>
+      <c r="D22" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="33">
+        <v>1</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="32"/>
@@ -1673,17 +1679,17 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="32"/>
-      <c r="D23" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="32">
-        <v>2025</v>
+      <c r="D23" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="33">
+        <v>1</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="32"/>
@@ -1701,17 +1707,17 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="32"/>
-      <c r="D24" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="32">
-        <v>2025</v>
+      <c r="D24" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="33">
+        <v>1</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
@@ -1729,17 +1735,17 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="32"/>
-      <c r="D25" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="32">
-        <v>2025</v>
+      <c r="D25" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="33">
+        <v>1</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
@@ -1757,17 +1763,17 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="32"/>
-      <c r="D26" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="32">
-        <v>2025</v>
+      <c r="D26" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="33">
+        <v>1</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
@@ -1784,17 +1790,17 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="32"/>
-      <c r="D27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="32">
-        <v>2025</v>
+      <c r="D27" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="33">
+        <v>1</v>
       </c>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
@@ -1821,8 +1827,8 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,8 +1836,8 @@
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="34" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
@@ -1844,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1853,7 +1859,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1865,16 +1871,16 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>2025</v>
+        <v>29</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="34">
+        <v>1</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1884,13 +1890,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>2025</v>
+        <v>24</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="34">
+        <v>1</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1900,13 +1906,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>2025</v>
+        <v>25</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="34">
+        <v>1</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1941,21 +1947,21 @@
   <sheetData>
     <row r="1" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" si="0">SUMIF($C$13:$C$24,$C2,E$13:E$24)</f>
@@ -1989,7 +1995,7 @@
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -2006,7 +2012,7 @@
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -2023,7 +2029,7 @@
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -2040,7 +2046,7 @@
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -2057,7 +2063,7 @@
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -2074,7 +2080,7 @@
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
@@ -2091,7 +2097,7 @@
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
@@ -2102,7 +2108,7 @@
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
@@ -2113,16 +2119,16 @@
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="H13" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
@@ -2145,7 +2151,7 @@
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2">
@@ -2163,7 +2169,7 @@
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16">
         <v>160</v>
@@ -2172,12 +2178,12 @@
         <v>215</v>
       </c>
       <c r="H16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2">
@@ -2195,7 +2201,7 @@
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="31">
@@ -2210,7 +2216,7 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="31">
@@ -2225,7 +2231,7 @@
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20">
         <v>1092</v>
@@ -2233,30 +2239,30 @@
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G21">
         <v>2465</v>
       </c>
       <c r="H21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="F26" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C27" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
@@ -2264,7 +2270,7 @@
     </row>
     <row r="28" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C28" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" s="15">
         <v>604.52757005392482</v>
@@ -2278,7 +2284,7 @@
     </row>
     <row r="29" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C29" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D29" s="15">
         <v>571.44501278772373</v>
@@ -2292,7 +2298,7 @@
     </row>
     <row r="30" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C30" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="15">
         <v>2055.5555555555557</v>
@@ -2306,7 +2312,7 @@
     </row>
     <row r="31" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C31" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31" s="15">
         <v>115.46511627906976</v>
@@ -2320,7 +2326,7 @@
     </row>
     <row r="32" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C32" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D32" s="15">
         <v>563.16159567275179</v>
@@ -2334,7 +2340,7 @@
     </row>
     <row r="33" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C33" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="9"/>
@@ -2342,7 +2348,7 @@
     </row>
     <row r="34" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C34" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" s="20">
         <v>1415.7024479470813</v>
@@ -2354,7 +2360,7 @@
     </row>
     <row r="35" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="15">
         <v>892.41336816762919</v>
@@ -2366,7 +2372,7 @@
     </row>
     <row r="36" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" s="15">
         <v>0</v>
@@ -2378,7 +2384,7 @@
     </row>
     <row r="37" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C37" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D37" s="15">
         <v>44.447058823529424</v>
@@ -2390,7 +2396,7 @@
     </row>
     <row r="38" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C38" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" s="15">
         <v>22.666666666666668</v>
@@ -2402,7 +2408,7 @@
     </row>
     <row r="39" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C39" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D39" s="24">
         <v>3.6555555555555554</v>
@@ -2414,7 +2420,7 @@
     </row>
     <row r="40" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C40" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D40" s="28">
         <v>6289.0399475094873</v>
@@ -2450,21 +2456,21 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <f>SUMIF($I$15:$I$33,$C2,E$15:E$33)</f>
@@ -2498,7 +2504,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -2515,7 +2521,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -2532,7 +2538,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -2549,7 +2555,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -2566,7 +2572,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
@@ -2576,7 +2582,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
@@ -2586,28 +2592,28 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
       </c>
       <c r="E15">
         <v>207.7</v>
@@ -2622,18 +2628,18 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>39</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
       </c>
       <c r="E16">
         <v>78.400000000000006</v>
@@ -2653,13 +2659,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17">
         <v>23.3</v>
@@ -2679,13 +2685,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18">
         <v>1083.5999999999999</v>
@@ -2705,13 +2711,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19">
         <v>75.925925925925924</v>
@@ -2720,18 +2726,18 @@
         <v>82</v>
       </c>
       <c r="I19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20">
         <v>1109.0740740740739</v>
@@ -2740,18 +2746,18 @@
         <v>1197.8</v>
       </c>
       <c r="I20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>46</v>
-      </c>
-      <c r="C21" t="s">
-        <v>47</v>
       </c>
       <c r="E21">
         <v>42.8</v>
@@ -2766,18 +2772,18 @@
         <v>1</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
       </c>
       <c r="E22">
         <v>111.6</v>
@@ -2792,18 +2798,18 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23">
         <v>37.9</v>
@@ -2818,18 +2824,18 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24">
         <v>257.2</v>
@@ -2844,18 +2850,18 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4">
@@ -2871,18 +2877,18 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4">
@@ -2898,18 +2904,18 @@
         <v>1.5764842840512225</v>
       </c>
       <c r="I26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C27" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4">
@@ -2925,18 +2931,18 @@
         <v>1.5834112149532713</v>
       </c>
       <c r="I27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" t="s">
         <v>48</v>
       </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28">
         <v>289.1556701030928</v>
@@ -2945,18 +2951,18 @@
         <v>274.7</v>
       </c>
       <c r="I28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E29">
         <v>394.94432989690722</v>
@@ -2965,18 +2971,18 @@
         <v>375.2</v>
       </c>
       <c r="I29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30">
         <v>366.3</v>
@@ -2985,18 +2991,18 @@
         <v>348</v>
       </c>
       <c r="I30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
         <v>48</v>
       </c>
-      <c r="B31" t="s">
-        <v>49</v>
-      </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E31">
         <v>976.8</v>
@@ -3005,18 +3011,18 @@
         <v>928</v>
       </c>
       <c r="I31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>61</v>
-      </c>
-      <c r="C32" t="s">
-        <v>62</v>
       </c>
       <c r="E32">
         <v>9</v>
@@ -3025,18 +3031,18 @@
         <v>8.5500000000000007</v>
       </c>
       <c r="I32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>64</v>
-      </c>
-      <c r="C33" t="s">
-        <v>65</v>
       </c>
       <c r="E33">
         <v>35</v>
@@ -3051,7 +3057,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3082,18 +3088,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E7" si="0">SUMIF($I$14:$I$32,$C2,E$14:E$32)</f>
@@ -3127,7 +3133,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -3144,7 +3150,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -3161,7 +3167,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -3178,7 +3184,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -3195,7 +3201,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
@@ -3206,7 +3212,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
@@ -3217,17 +3223,17 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>6</v>
@@ -3235,13 +3241,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
         <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
       </c>
       <c r="E14">
         <v>96.2</v>
@@ -3256,18 +3262,18 @@
         <v>2.3811518944574046</v>
       </c>
       <c r="I14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
         <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
       </c>
       <c r="E15">
         <v>464.6</v>
@@ -3287,13 +3293,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E16">
         <v>55.55555555555555</v>
@@ -3302,18 +3308,18 @@
         <v>60</v>
       </c>
       <c r="I16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17">
         <v>1387.9629629629628</v>
@@ -3322,18 +3328,18 @@
         <v>1499</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18">
         <v>254.84241823587709</v>
@@ -3353,13 +3359,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
         <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>75</v>
       </c>
       <c r="E19">
         <v>348.8</v>
@@ -3374,18 +3380,18 @@
         <v>1.9926075268817205</v>
       </c>
       <c r="I19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20">
         <v>146</v>
@@ -3400,18 +3406,18 @@
         <v>2.4924139862751513</v>
       </c>
       <c r="I20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21">
         <v>89.1</v>
@@ -3426,18 +3432,18 @@
         <v>2.0999908096682289</v>
       </c>
       <c r="I21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E22">
         <v>1053.4000000000001</v>
@@ -3452,18 +3458,18 @@
         <v>2.5236559139784944</v>
       </c>
       <c r="I22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23">
         <v>784.5</v>
@@ -3475,18 +3481,18 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24">
         <v>1578.9</v>
@@ -3498,18 +3504,18 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25">
         <v>217</v>
@@ -3524,18 +3530,18 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26">
         <v>2714.7376106882089</v>
@@ -3544,18 +3550,18 @@
         <v>2742</v>
       </c>
       <c r="I26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27">
         <v>3658.2623893117911</v>
@@ -3564,18 +3570,18 @@
         <v>3695</v>
       </c>
       <c r="I27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
         <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
       </c>
       <c r="E28">
         <v>753.2</v>
@@ -3590,18 +3596,18 @@
         <v>3.1333333333333333</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
         <v>86</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
       </c>
       <c r="E29">
         <v>80</v>
@@ -3616,18 +3622,18 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4">
@@ -3641,21 +3647,21 @@
       </c>
       <c r="H30" s="4"/>
       <c r="I30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E31">
         <v>69.824248430789552</v>
@@ -3670,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>